<commit_message>
Add client count and remove row 3 in Excel export
</commit_message>
<xml_diff>
--- a/Public/upload/Export n table Client.xlsx
+++ b/Public/upload/Export n table Client.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Feuille1"/>
+    <sheet name="Feuille1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>LISTE CLIENTS</t>
   </si>
@@ -106,33 +107,38 @@
     <t>Albi</t>
   </si>
   <si>
-    <t>CLT879644</t>
+    <t>Nombre Clients :</t>
+  </si>
+  <si>
+    <t>Nombre Clients = 10</t>
   </si>
   <si>
     <t>Marie Brigitte</t>
-  </si>
-  <si>
-    <t>Nombre Clients :</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -144,16 +150,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffff00"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFb4c7dc"/>
+        <fgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -161,50 +169,32 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFc6c6c6"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFc6c6c6"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFc6c6c6"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+  <cellXfs count="4">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -213,10 +203,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -254,71 +244,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -342,53 +332,54 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="51000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
+                <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
+                <a:shade val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="9500"/>
+              <a:shade val="95000"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -398,7 +389,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -407,7 +398,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -416,7 +407,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -424,10 +415,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -456,7 +447,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="20000"/>
+                <a:shade val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -469,12 +460,13 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
+                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -492,29 +484,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="0"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" showGridLines="true" showRowColHeaders="1" topLeftCell="A1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="11.53515625" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="40.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="33.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" width="14.06" customWidth="true" style="0"/>
+    <col min="3" max="3" width="13.99" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="22.5">
+    <row r="1" spans="1:3" customHeight="1" ht="17.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="22.5">
+    <row r="2" spans="1:3" customHeight="1" ht="17.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -525,128 +518,135 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:3"/>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="3" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="3" t="s">
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="3" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" customHeight="1" ht="17.35">
+      <c r="A14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="22.5">
-      <c r="A13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.0527777777778" bottom="1.0527777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="1" useFirstPageNumber="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Client model and fix formatting in ExcelController
</commit_message>
<xml_diff>
--- a/Public/upload/Export n table Client.xlsx
+++ b/Public/upload/Export n table Client.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>LISTE CLIENTS</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>Albi</t>
-  </si>
-  <si>
-    <t>Nombre Clients :</t>
   </si>
   <si>
     <t>Nombre Clients = 10</t>
@@ -519,127 +516,125 @@
       </c>
     </row>
     <row r="3" spans="1:3"/>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" customHeight="1" ht="17.35">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" customHeight="1" ht="17.35">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" customHeight="1" ht="17.35">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3" customHeight="1" ht="17.35">
+      <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:3" customHeight="1" ht="17.35">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:3" customHeight="1" ht="17.35">
+      <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" customHeight="1" ht="17.35">
+      <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:3" customHeight="1" ht="17.35">
+      <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:3" customHeight="1" ht="17.35">
+      <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:3" customHeight="1" ht="17.35">
+      <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" customHeight="1" ht="17.35">
-      <c r="A14" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7875" right="0.7875" top="1.0527777777778" bottom="1.0527777777778" header="0.7875" footer="0.7875"/>

</xml_diff>